<commit_message>
fixed and added more OMs PDF's
</commit_message>
<xml_diff>
--- a/Open-OMs.xlsx
+++ b/Open-OMs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5190806</t>
+          <t>5191638</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -462,7 +462,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5191829</t>
+          <t>685601336053</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -473,10 +473,721 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>685601337781</t>
+          <t>685601351429</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5192407</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>685601351883</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>685601347597</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>685601357432</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5193183</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5192919</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5192920</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5192915</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5192914</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>685601352518</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>685601349125</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>68560132676705082024</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5192400</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>685601351966</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5191494</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>685601350457</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5192253</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5190399</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5193017</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>519298015012025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5193045</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>685601354903</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>685601352367</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5190757</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>685601352936</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5192793</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>685601350929</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>5192923</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>5192651</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>5192836</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>5191946</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>685601346254</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>685601351259</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>685601351533</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>685601351260</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>685601351264</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>685601341400</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>5192403</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>685601352369</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>685601351399</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>685601350929</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>5192751</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>5192548</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>5192472</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>685601348892</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>685601349239</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>685601330195</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>685601341718</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>685601341513</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>685601340208</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>685601351893</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>5190918</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>5191870</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>685601350457</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>5191946</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>5192402</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>5192313</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>5192397</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>685601340175</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>685601347570</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>541</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>5190726</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>5192558</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>5191646</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: new bot created
</commit_message>
<xml_diff>
--- a/Open-OMs.xlsx
+++ b/Open-OMs.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAACB8C1-553F-4451-80F0-2D1787B5F0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE8CEC5-F085-4080-B19C-D27EF52F8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>OM</t>
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Encerrado!</t>
+  </si>
+  <si>
+    <t>Ordem pendente!</t>
   </si>
 </sst>
 </file>
@@ -43,10 +52,8 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,13 +91,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -110,9 +120,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -150,7 +160,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -184,7 +194,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -219,10 +228,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -399,487 +407,597 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>5192057</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>685601359764</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>685601354371</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>5193772</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>5193561</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>5193808</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>5193211</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>5193463</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>5192325</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>5191530</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>685601355410</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>5193408</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>685601356153</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>685601355231</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>5193632</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>685601359092</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>685601338183</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>5193446</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>5193374</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>5193338</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="2">
         <v>5191218</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>685601350660</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>685601357000</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>5193455</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>5193504</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>685601356136</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>685601354475</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>5191740</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>5193508</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>685601357498</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>5193570</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>685601356832</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>685601356831</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>685601359197</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>685601356833</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" s="2">
         <v>685601359200</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>685601359199</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="2">
         <v>685601357145</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" s="2">
         <v>685601356828</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="2">
         <v>685601359195</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="2">
         <v>685601359198</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>685601359196</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>685601356839</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="2">
         <v>685601356836</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" s="2">
         <v>685601356840</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="2">
         <v>685601356838</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" s="2">
         <v>685601356834</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" s="2">
         <v>5193506</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" s="2">
         <v>5193336</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" s="2">
         <v>5193453</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" s="2">
         <v>685601355230</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" s="2">
         <v>685601359645</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" s="2">
         <v>5193204</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" s="2">
         <v>5191160</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" s="2">
         <v>5191630</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" s="2">
         <v>5190853</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" s="2">
         <v>685601356155</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" s="2">
         <v>685601355371</v>
       </c>
+      <c r="C59" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: pdf readers updated
</commit_message>
<xml_diff>
--- a/Open-OMs.xlsx
+++ b/Open-OMs.xlsx
@@ -1,81 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEC85EC-7E95-4B7E-B295-535390C0EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>OM</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>685601371216</t>
-  </si>
-  <si>
-    <t>685601362435</t>
-  </si>
-  <si>
-    <t>685601368700</t>
-  </si>
-  <si>
-    <t>685601370633</t>
-  </si>
-  <si>
-    <t>685601370632</t>
-  </si>
-  <si>
-    <t>685601375762</t>
-  </si>
-  <si>
-    <t>685601374529</t>
-  </si>
-  <si>
-    <t>685601372066</t>
-  </si>
-  <si>
-    <t>685601371261</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,73 +420,286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>685601352106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5197000</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>5196576</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5196597</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5196705</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5196234</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5196126</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>5194999</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5196304</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5196368</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5196706</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>5196606</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5196606</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5194692</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5194685</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>5194688</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5196552</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5196718</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>5196365</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>5195945</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>685601375584</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>685601374537</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>685601371530</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>685601380532</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>685601371845</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>685601366313</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>685601376800</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>685601379042</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>685601370984</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>685601370982</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>685601374833</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>685601377972</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>685601377854</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
used: finish-LP and OM used
</commit_message>
<xml_diff>
--- a/Open-OMs.xlsx
+++ b/Open-OMs.xlsx
@@ -446,260 +446,324 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>5197072</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>5197072</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>5197173</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>5197173</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>5196791</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>5196791</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>5197351</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>5197351</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5197174</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>5197174</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5196603</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>5196603</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>5196895</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="A8" t="n">
+        <v>5196895</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>5196780</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="A9" t="n">
+        <v>5196780</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>5197447</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="A10" t="n">
+        <v>5197447</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>5196812</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="A11" t="n">
+        <v>5196812</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>5197114</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="A12" t="n">
+        <v>5197114</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>5197572</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="A13" t="n">
+        <v>5197572</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ordem pendente!</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>685601370003</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="A14" t="n">
+        <v>685601370003</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>685601380872</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="A15" t="n">
+        <v>685601380872</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>685601374545</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="A16" t="n">
+        <v>685601374545</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>685601378879</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="A17" t="n">
+        <v>685601378879</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>685601378435</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="A18" t="n">
+        <v>685601378435</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>685601378437</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="A19" t="n">
+        <v>685601378437</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>685601377298</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="A20" t="n">
+        <v>685601377298</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>685601382621</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="A21" t="n">
+        <v>685601382621</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>685601381340</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="A22" t="n">
+        <v>685601381340</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>685601367925</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="A23" t="n">
+        <v>685601367925</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>685601378723</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="A24" t="n">
+        <v>685601378723</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>685601378307</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="A25" t="n">
+        <v>685601378307</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>685601383769</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="A26" t="n">
+        <v>685601383769</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>685601355769</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="A27" t="n">
+        <v>685601355769</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ordem pendente!</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>685601375759</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>685601375759</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>685601375604</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="A29" t="n">
+        <v>685601375604</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>685601370724</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="A30" t="n">
+        <v>685601370724</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>685601378491</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="A31" t="n">
+        <v>685601378491</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>685601364160</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="A32" t="n">
+        <v>685601364160</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Ordem pendente!</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>685601377899</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="A33" t="n">
+        <v>685601377899</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: bot text updated, finish LP and OM used
</commit_message>
<xml_diff>
--- a/Open-OMs.xlsx
+++ b/Open-OMs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,244 +446,54 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>5197765</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>5197633</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ordem pendente!</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>5197830</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>685601367443</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>5197796</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>685601368494</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>5197244</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>685601382620</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5197784</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5197689</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>5197633</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>5196771</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>5197378</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>5197312</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>5197225</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>5197309</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>685601375964</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>685601378213</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>685601374947</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>685601381931</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>685601380722</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>685601371495</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>685601378812</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>685601382675</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>685601378646</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>685601377886</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>685601382704</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>685601382419</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>685601376660</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>685601359848</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>685601367443</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>685601368494</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>685601382620</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>685601375585</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>685601375585</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>